<commit_message>
Update Danh sách thành viên
</commit_message>
<xml_diff>
--- a/Member/DanhSachThanhVien.xlsx
+++ b/Member/DanhSachThanhVien.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>MSSV</t>
   </si>
@@ -22,6 +22,9 @@
     <t>Email</t>
   </si>
   <si>
+    <t>Tài khoản Github</t>
+  </si>
+  <si>
     <t>Số ĐT</t>
   </si>
   <si>
@@ -40,6 +43,9 @@
     <t>1212100@student.hcmus.edu.vn</t>
   </si>
   <si>
+    <t>dtgianggithub</t>
+  </si>
+  <si>
     <t>Project Manager</t>
   </si>
   <si>
@@ -73,6 +79,9 @@
     <t>mrthien30@gmail.com</t>
   </si>
   <si>
+    <t>Thiện 1212381</t>
+  </si>
+  <si>
     <t>Developer</t>
   </si>
   <si>
@@ -101,26 +110,48 @@
   </si>
   <si>
     <t>Đồ án môn học, thực tập</t>
+  </si>
+  <si>
+    <t>Nguyễn Thành Toàn</t>
+  </si>
+  <si>
+    <t>nguyenthanhtoan_94@yahoo.com</t>
+  </si>
+  <si>
+    <t>nguyenthanhtoan</t>
+  </si>
+  <si>
+    <t>0975178324</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FF141823"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F7F8"/>
+        <bgColor rgb="FFF6F7F8"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -134,12 +165,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -161,10 +195,12 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="3" max="3" width="30.57"/>
-    <col customWidth="1" min="4" max="5" width="31.57"/>
-    <col customWidth="1" min="6" max="6" width="18.0"/>
-    <col customWidth="1" min="7" max="7" width="94.29"/>
-    <col customWidth="1" min="8" max="8" width="37.86"/>
+    <col customWidth="1" min="4" max="4" width="31.57"/>
+    <col customWidth="1" min="5" max="5" width="27.0"/>
+    <col customWidth="1" min="6" max="6" width="31.57"/>
+    <col customWidth="1" min="7" max="7" width="18.0"/>
+    <col customWidth="1" min="8" max="8" width="94.29"/>
+    <col customWidth="1" min="9" max="9" width="37.86"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -189,26 +225,34 @@
       <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="1">
         <v>1212100.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.688452784E9</v>
+      </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -216,22 +260,25 @@
         <v>1212508.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5">
@@ -239,17 +286,20 @@
         <v>1212381.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6">
@@ -257,16 +307,19 @@
         <v>1212297.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -274,22 +327,42 @@
         <v>1212117.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="1">
+        <v>30</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="1">
         <v>1.646280957E9</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="1">
+        <v>1212420.0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>